<commit_message>
going back to normal python, but keeping the type annotations. Cython isnt helpful bc im using alot of objects versus just pure numbers
</commit_message>
<xml_diff>
--- a/SWAT Schedule Apr 14, Sunday.xlsx
+++ b/SWAT Schedule Apr 14, Sunday.xlsx
@@ -142,67 +142,67 @@
     <t>SERVE</t>
   </si>
   <si>
+    <t>KSWAT3</t>
+  </si>
+  <si>
+    <t>GIRLS GROTTO</t>
+  </si>
+  <si>
+    <t>HALF STAFF</t>
+  </si>
+  <si>
+    <t>FLAG UP</t>
+  </si>
+  <si>
     <t>CAMP STORE</t>
   </si>
   <si>
+    <t>POOL</t>
+  </si>
+  <si>
+    <t>DH</t>
+  </si>
+  <si>
+    <t>BOYS GROTTO</t>
+  </si>
+  <si>
+    <t>OFFICE</t>
+  </si>
+  <si>
+    <t>WATER RUN</t>
+  </si>
+  <si>
+    <t>BARRET</t>
+  </si>
+  <si>
+    <t>KSWAT2</t>
+  </si>
+  <si>
+    <t>CLODGE</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
     <t>TRASH WATER</t>
   </si>
   <si>
-    <t>HALF STAFF</t>
-  </si>
-  <si>
-    <t>FLAG UP</t>
-  </si>
-  <si>
-    <t>DH</t>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>PAV</t>
+  </si>
+  <si>
+    <t>SLOUNGE</t>
+  </si>
+  <si>
+    <t>GIRLS BATH</t>
+  </si>
+  <si>
+    <t>CHAPEL</t>
   </si>
   <si>
     <t>BOYS BATH</t>
-  </si>
-  <si>
-    <t>GIRLS GROTTO</t>
-  </si>
-  <si>
-    <t>WATER RUN</t>
-  </si>
-  <si>
-    <t>SLOUNGE</t>
-  </si>
-  <si>
-    <t>KSWAT2</t>
-  </si>
-  <si>
-    <t>POOL</t>
-  </si>
-  <si>
-    <t>CHAPEL</t>
-  </si>
-  <si>
-    <t>KSWAT3</t>
-  </si>
-  <si>
-    <t>PAC</t>
-  </si>
-  <si>
-    <t>BARRET</t>
-  </si>
-  <si>
-    <t>CLODGE</t>
-  </si>
-  <si>
-    <t>GIRLS BATH</t>
-  </si>
-  <si>
-    <t>BOYS GROTTO</t>
-  </si>
-  <si>
-    <t>PAV</t>
-  </si>
-  <si>
-    <t>HC</t>
-  </si>
-  <si>
-    <t>OFFICE</t>
   </si>
   <si>
     <t>SCHEDULE</t>
@@ -295,12 +295,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC9DAF8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF4CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -308,6 +302,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -742,10 +742,13 @@
       <c r="H5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="Q5" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -756,16 +759,19 @@
       <c r="C6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="D6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -773,42 +779,51 @@
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>48</v>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="Q7" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="L8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -816,17 +831,20 @@
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>46</v>
+      <c r="B9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -836,19 +854,16 @@
       <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="Q10" s="9" t="s">
+      <c r="D10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -856,13 +871,22 @@
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="H11" s="9" t="s">
+      <c r="C11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10" t="s">
         <v>46</v>
       </c>
     </row>
@@ -870,72 +894,66 @@
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="K12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>53</v>
+      <c r="C12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="Q13" s="9" t="s">
-        <v>43</v>
+      <c r="C13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="Q13" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>55</v>
+      <c r="Q14" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -945,290 +963,272 @@
       <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="D15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>42</v>
+      <c r="Q15" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>56</v>
+      <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="H16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L17" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q18" s="9" t="s">
-        <v>58</v>
+      <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="C19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="Q20" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>42</v>
+      <c r="Q21" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="8" t="s">
+      <c r="C22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q22" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="Q23" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="9" t="s">
+      <c r="K24" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="Q24" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q25" s="9" t="s">
-        <v>62</v>
+      <c r="C25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="B26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L26" s="8" t="s">
-        <v>42</v>
+      <c r="Q26" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>42</v>
+      <c r="C27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1239,13 +1239,13 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J22:M22"/>
     <mergeCell ref="B2:Q3"/>
     <mergeCell ref="A28:Q28"/>
   </mergeCells>

</xml_diff>